<commit_message>
added aes .dat-file from Staib DESA
</commit_message>
<xml_diff>
--- a/test/1_lab_journal.xlsx
+++ b/test/1_lab_journal.xlsx
@@ -196,7 +196,7 @@
     <t xml:space="preserve">HOPG</t>
   </si>
   <si>
-    <t xml:space="preserve">STM RHK SM4</t>
+    <t xml:space="preserve">STM RHK SM4 .sm4 file</t>
   </si>
   <si>
     <t xml:space="preserve">19.10.2021</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">aes</t>
   </si>
   <si>
-    <t xml:space="preserve">AES Staib DESA</t>
+    <t xml:space="preserve">AES Staib DESA .dat file</t>
   </si>
 </sst>
 </file>
@@ -363,10 +363,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20"/>

</xml_diff>

<commit_message>
implemented support for Nanonis sxm-files
</commit_message>
<xml_diff>
--- a/test/1_lab_journal.xlsx
+++ b/test/1_lab_journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t xml:space="preserve">AES Staib DESA .dat file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.10.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stm-nanonis-sxm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM Nanonis .sxm file</t>
   </si>
 </sst>
 </file>
@@ -363,10 +372,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20"/>
@@ -834,8 +843,19 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2"/>

</xml_diff>